<commit_message>
revison to correct a data error
</commit_message>
<xml_diff>
--- a/ResultsByUHF20230823/DailyProjections_citywide20230823.xlsx
+++ b/ResultsByUHF20230823/DailyProjections_citywide20230823.xlsx
@@ -458,57 +458,57 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4403 (2320, 7490)</t>
+          <t>7604 (4171, 12420)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>192 (114, 304)</t>
+          <t>358 (226, 536)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>28 (16, 50)</t>
+          <t>58 (33, 100)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>21 (10, 41)</t>
+          <t>44 (21, 83)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>44 (26, 71)</t>
+          <t>87 (54, 136)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>36 (20, 61)</t>
+          <t>73 (41, 119)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 21)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -535,57 +535,57 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4223 (2395, 7184)</t>
+          <t>7305 (4315, 11897)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>192 (116, 301)</t>
+          <t>351 (224, 526)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>27 (15, 48)</t>
+          <t>55 (31, 96)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>20 (9, 39)</t>
+          <t>42 (19, 80)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>12 (7, 20)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>42 (25, 69)</t>
+          <t>85 (52, 134)</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>35 (19, 60)</t>
+          <t>71 (39, 117)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 21)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -612,57 +612,57 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4087 (2425, 7147)</t>
+          <t>7059 (4344, 11786)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>193 (118, 301)</t>
+          <t>348 (226, 519)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>25 (14, 47)</t>
+          <t>52 (29, 93)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>19 (9, 38)</t>
+          <t>40 (19, 77)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>41 (24, 68)</t>
+          <t>82 (50, 131)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>34 (18, 59)</t>
+          <t>68 (37, 114)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 21)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -689,57 +689,57 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>3988 (2423, 7220)</t>
+          <t>6870 (4325, 11815)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>194 (120, 302)</t>
+          <t>347 (226, 516)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>25 (14, 45)</t>
+          <t>51 (29, 91)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>19 (9, 38)</t>
+          <t>39 (19, 75)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 18)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>4 (3, 7)</t>
+          <t>9 (5, 14)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>39 (23, 66)</t>
+          <t>79 (47, 129)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>32 (17, 57)</t>
+          <t>65 (35, 112)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 17)</t>
         </is>
       </c>
     </row>
@@ -766,57 +766,57 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>3924 (2402, 7328)</t>
+          <t>6740 (4275, 11857)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>195 (121, 303)</t>
+          <t>345 (225, 514)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>25 (14, 45)</t>
+          <t>50 (28, 89)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>19 (9, 37)</t>
+          <t>39 (19, 74)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 17)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
+          <t>8 (5, 14)</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
           <t>4 (2, 7)</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>3 (1, 4)</t>
-        </is>
-      </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>38 (22, 64)</t>
+          <t>76 (45, 125)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>31 (15, 55)</t>
+          <t>62 (32, 109)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>6 (4, 11)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 17)</t>
         </is>
       </c>
     </row>
@@ -843,57 +843,57 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3888 (2380, 7441)</t>
+          <t>6652 (4212, 11933)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>195 (122, 304)</t>
+          <t>343 (223, 511)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>24 (14, 45)</t>
+          <t>49 (28, 88)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>19 (9, 37)</t>
+          <t>39 (19, 74)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>8 (4, 13)</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>4 (2, 7)</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>36 (20, 62)</t>
+          <t>73 (42, 122)</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>29 (15, 54)</t>
+          <t>60 (30, 105)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>12 (7, 20)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -920,57 +920,57 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3870 (2348, 7561)</t>
+          <t>6589 (4151, 12007)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>194 (121, 305)</t>
+          <t>340 (222, 509)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>24 (13, 45)</t>
+          <t>49 (27, 87)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>19 (9, 38)</t>
+          <t>39 (19, 74)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>4 (2, 6)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>34 (19, 61)</t>
+          <t>70 (40, 118)</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>28 (14, 52)</t>
+          <t>57 (28, 102)</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -997,57 +997,57 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3875 (2322, 7702)</t>
+          <t>6564 (4087, 12093)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>194 (122, 306)</t>
+          <t>337 (221, 506)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>24 (13, 45)</t>
+          <t>48 (27, 87)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>20 (10, 38)</t>
+          <t>39 (20, 74)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4 (2, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>3 (2, 6)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>4 (2, 6)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>33 (18, 59)</t>
+          <t>67 (38, 115)</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>26 (13, 50)</t>
+          <t>54 (27, 99)</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -1074,57 +1074,57 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3892 (2298, 7848)</t>
+          <t>6560 (4037, 12195)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>193 (121, 308)</t>
+          <t>335 (219, 504)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>24 (13, 46)</t>
+          <t>48 (27, 87)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>20 (10, 39)</t>
+          <t>39 (20, 74)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (5, 14)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>3 (2, 6)</t>
+          <t>6 (4, 11)</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>4 (2, 6)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>31 (17, 57)</t>
+          <t>64 (36, 111)</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>25 (12, 49)</t>
+          <t>52 (25, 96)</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>11 (6, 18)</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
     </row>
@@ -1151,57 +1151,57 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3912 (2275, 8008)</t>
+          <t>6554 (3984, 12302)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>193 (121, 310)</t>
+          <t>332 (218, 503)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>24 (13, 46)</t>
+          <t>48 (27, 87)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>20 (10, 39)</t>
+          <t>39 (20, 75)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 14)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>3 (2, 6)</t>
+          <t>6 (3, 11)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>4 (2, 6)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>30 (17, 55)</t>
+          <t>61 (34, 108)</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>49 (24, 93)</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 18)</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>4 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
     </row>
@@ -1228,57 +1228,57 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3944 (2251, 8157)</t>
+          <t>6555 (3933, 12394)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>193 (120, 312)</t>
+          <t>330 (216, 503)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>24 (13, 47)</t>
+          <t>47 (26, 87)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>20 (10, 40)</t>
+          <t>39 (20, 75)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
+          <t>6 (3, 11)</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>29 (16, 54)</t>
+          <t>59 (33, 105)</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>23 (11, 46)</t>
+          <t>48 (23, 90)</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 17)</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (5, 14)</t>
         </is>
       </c>
     </row>
@@ -1305,57 +1305,57 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>3972 (2225, 8310)</t>
+          <t>6566 (3885, 12487)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>193 (120, 316)</t>
+          <t>328 (214, 504)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>24 (13, 47)</t>
+          <t>47 (26, 88)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>20 (10, 41)</t>
+          <t>39 (20, 75)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
+          <t>6 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>28 (15, 53)</t>
+          <t>57 (32, 102)</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>23 (11, 45)</t>
+          <t>46 (23, 88)</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (5, 17)</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 14)</t>
         </is>
       </c>
     </row>
@@ -1382,57 +1382,57 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>4010 (2208, 8462)</t>
+          <t>6575 (3843, 12577)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>193 (119, 320)</t>
+          <t>326 (212, 505)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>24 (13, 48)</t>
+          <t>47 (26, 88)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>20 (10, 41)</t>
+          <t>39 (20, 76)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>3 (2, 5)</t>
+          <t>5 (3, 10)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>3 (2, 6)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>27 (15, 52)</t>
+          <t>55 (31, 100)</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>22 (11, 44)</t>
+          <t>45 (22, 86)</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>9 (5, 16)</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 13)</t>
         </is>
       </c>
     </row>
@@ -1459,57 +1459,57 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4047 (2188, 8612)</t>
+          <t>6589 (3800, 12666)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>193 (118, 324)</t>
+          <t>325 (210, 506)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>24 (13, 49)</t>
+          <t>46 (26, 89)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>39 (20, 76)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
+          <t>5 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>27 (15, 51)</t>
+          <t>54 (30, 98)</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>22 (10, 43)</t>
+          <t>44 (22, 84)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 16)</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
     </row>
@@ -1536,57 +1536,57 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4150 (2205, 7048)</t>
+          <t>7243 (3972, 11848)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>184 (110, 291)</t>
+          <t>336 (216, 501)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>30 (17, 53)</t>
+          <t>60 (35, 105)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>23 (11, 44)</t>
+          <t>47 (23, 87)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 16)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>46 (28, 74)</t>
+          <t>90 (56, 139)</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>38 (21, 64)</t>
+          <t>76 (43, 122)</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>14 (8, 21)</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -1613,57 +1613,57 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>3983 (2274, 6749)</t>
+          <t>6955 (4067, 11353)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>183 (111, 289)</t>
+          <t>329 (214, 492)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>28 (15, 51)</t>
+          <t>57 (32, 100)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>21 (10, 42)</t>
+          <t>44 (21, 84)</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>44 (27, 72)</t>
+          <t>88 (54, 137)</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>37 (20, 63)</t>
+          <t>73 (41, 120)</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>14 (8, 21)</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -1690,57 +1690,57 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3851 (2296, 6690)</t>
+          <t>6706 (4078, 11225)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>183 (113, 288)</t>
+          <t>327 (214, 487)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>27 (15, 49)</t>
+          <t>54 (30, 97)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>21 (9, 41)</t>
+          <t>42 (20, 81)</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (6, 15)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>3 (1, 5)</t>
+          <t>4 (2, 7)</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>43 (25, 71)</t>
+          <t>85 (52, 134)</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>35 (19, 61)</t>
+          <t>71 (39, 117)</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>14 (8, 21)</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -1767,57 +1767,57 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>3753 (2290, 6735)</t>
+          <t>6513 (4042, 11212)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>184 (114, 288)</t>
+          <t>325 (213, 484)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>26 (15, 48)</t>
+          <t>53 (29, 94)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>20 (9, 40)</t>
+          <t>41 (19, 79)</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 18)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>4 (3, 8)</t>
+          <t>9 (5, 14)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2 (1, 5)</t>
+          <t>4 (2, 6)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>41 (24, 69)</t>
+          <t>82 (49, 131)</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>34 (18, 60)</t>
+          <t>68 (36, 114)</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 21)</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>6 (3, 9)</t>
+          <t>11 (7, 17)</t>
         </is>
       </c>
     </row>
@@ -1844,57 +1844,57 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>3687 (2274, 6812)</t>
+          <t>6368 (3988, 11230)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>184 (114, 289)</t>
+          <t>322 (211, 481)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>26 (14, 47)</t>
+          <t>51 (29, 92)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>20 (10, 39)</t>
+          <t>40 (19, 77)</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 17)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (5, 14)</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>4 (2, 6)</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>40 (23, 67)</t>
+          <t>78 (47, 128)</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>32 (16, 58)</t>
+          <t>64 (34, 111)</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>7 (4, 11)</t>
+          <t>13 (8, 20)</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 17)</t>
         </is>
       </c>
     </row>
@@ -1921,57 +1921,57 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3648 (2244, 6897)</t>
+          <t>6263 (3915, 11265)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>183 (114, 289)</t>
+          <t>319 (208, 478)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>25 (14, 47)</t>
+          <t>50 (28, 91)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>20 (10, 39)</t>
+          <t>40 (19, 76)</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 13)</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>3 (2, 6)</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>38 (22, 65)</t>
+          <t>75 (44, 124)</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>31 (15, 56)</t>
+          <t>61 (32, 108)</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>6 (4, 11)</t>
+          <t>13 (7, 20)</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>11 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -1998,57 +1998,57 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>3625 (2213, 6999)</t>
+          <t>6187 (3843, 11288)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>182 (113, 289)</t>
+          <t>316 (206, 474)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>25 (14, 46)</t>
+          <t>49 (27, 90)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>20 (10, 39)</t>
+          <t>40 (19, 76)</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>3 (2, 6)</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>36 (20, 64)</t>
+          <t>72 (42, 120)</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>29 (14, 55)</t>
+          <t>58 (30, 104)</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>6 (4, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -2075,57 +2075,57 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3615 (2176, 7098)</t>
+          <t>6135 (3775, 11346)</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>181 (113, 288)</t>
+          <t>312 (204, 471)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>25 (14, 47)</t>
+          <t>49 (27, 89)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>20 (10, 40)</t>
+          <t>39 (19, 76)</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>4 (2, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>4 (2, 6)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2 (1, 4)</t>
+          <t>3 (2, 6)</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>35 (19, 62)</t>
+          <t>69 (39, 117)</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>28 (14, 53)</t>
+          <t>56 (28, 101)</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>12 (7, 19)</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>10 (6, 16)</t>
         </is>
       </c>
     </row>
@@ -2152,57 +2152,57 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3613 (2145, 7208)</t>
+          <t>6096 (3702, 11388)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>180 (112, 289)</t>
+          <t>309 (202, 468)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>25 (14, 47)</t>
+          <t>48 (26, 89)</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>20 (10, 40)</t>
+          <t>39 (19, 76)</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4 (2, 8)</t>
+          <t>8 (5, 14)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
+          <t>6 (4, 11)</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>33 (18, 60)</t>
+          <t>66 (37, 113)</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>27 (13, 51)</t>
+          <t>53 (26, 98)</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>11 (7, 18)</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
     </row>
@@ -2229,57 +2229,57 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>3619 (2118, 7312)</t>
+          <t>6061 (3638, 11420)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>179 (112, 290)</t>
+          <t>306 (200, 466)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>25 (14, 47)</t>
+          <t>47 (26, 88)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>20 (10, 40)</t>
+          <t>39 (19, 75)</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 13)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
+          <t>6 (3, 11)</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>32 (17, 58)</t>
+          <t>63 (35, 110)</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>26 (12, 50)</t>
+          <t>51 (25, 95)</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>6 (3, 10)</t>
+          <t>11 (6, 18)</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>5 (3, 8)</t>
+          <t>9 (5, 15)</t>
         </is>
       </c>
     </row>
@@ -2306,57 +2306,57 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>3628 (2086, 7430)</t>
+          <t>6040 (3576, 11468)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>178 (111, 292)</t>
+          <t>303 (198, 464)</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>25 (13, 48)</t>
+          <t>47 (25, 88)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>20 (10, 41)</t>
+          <t>39 (19, 75)</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
+          <t>6 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>31 (17, 57)</t>
+          <t>61 (34, 107)</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>25 (12, 48)</t>
+          <t>49 (24, 92)</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 17)</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>4 (2, 8)</t>
+          <t>9 (5, 14)</t>
         </is>
       </c>
     </row>
@@ -2383,57 +2383,57 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>3641 (2057, 7534)</t>
+          <t>6023 (3518, 11511)</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>177 (110, 294)</t>
+          <t>300 (195, 463)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>24 (13, 48)</t>
+          <t>46 (25, 87)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>20 (10, 41)</t>
+          <t>38 (19, 75)</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 13)</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
+          <t>6 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>30 (16, 55)</t>
+          <t>58 (32, 105)</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>47 (23, 90)</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>10 (6, 17)</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (5, 14)</t>
         </is>
       </c>
     </row>
@@ -2460,57 +2460,57 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>3654 (2030, 7649)</t>
+          <t>6000 (3459, 11542)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>177 (108, 296)</t>
+          <t>297 (192, 462)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>24 (13, 48)</t>
+          <t>45 (25, 87)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>38 (19, 75)</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>5 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>29 (16, 54)</t>
+          <t>56 (31, 102)</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>23 (11, 46)</t>
+          <t>46 (22, 88)</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>9 (5, 16)</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>8 (4, 13)</t>
         </is>
       </c>
     </row>
@@ -2537,57 +2537,57 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3669 (2006, 7757)</t>
+          <t>5985 (3407, 11572)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>176 (107, 299)</t>
+          <t>294 (189, 462)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>24 (13, 49)</t>
+          <t>45 (24, 87)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>37 (19, 75)</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
+          <t>5 (3, 10)</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
           <t>3 (2, 6)</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>2 (1, 4)</t>
-        </is>
-      </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>28 (15, 53)</t>
+          <t>55 (30, 100)</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>23 (11, 45)</t>
+          <t>44 (22, 86)</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>5 (3, 9)</t>
+          <t>9 (5, 16)</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>4 (2, 7)</t>
+          <t>7 (4, 12)</t>
         </is>
       </c>
     </row>
@@ -2689,42 +2689,42 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>260 (117, 539)</t>
+          <t>547 (253, 1100)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>213 (79, 481)</t>
+          <t>454 (178, 989)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>35 (14, 76)</t>
+          <t>69 (29, 146)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>32 (16, 58)</t>
+          <t>64 (34, 114)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>260 (117, 539)</t>
+          <t>547 (253, 1100)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>213 (79, 481)</t>
+          <t>454 (178, 989)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>35 (14, 76)</t>
+          <t>69 (29, 146)</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>32 (16, 58)</t>
+          <t>64 (34, 114)</t>
         </is>
       </c>
     </row>
@@ -2751,42 +2751,42 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>244 (108, 518)</t>
+          <t>516 (234, 1059)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>198 (72, 460)</t>
+          <t>425 (161, 948)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>34 (14, 75)</t>
+          <t>67 (28, 145)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>31 (16, 57)</t>
+          <t>63 (33, 113)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>244 (108, 518)</t>
+          <t>516 (234, 1059)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>198 (72, 460)</t>
+          <t>425 (161, 948)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>34 (14, 75)</t>
+          <t>67 (28, 145)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>31 (16, 57)</t>
+          <t>63 (33, 113)</t>
         </is>
       </c>
     </row>
@@ -2813,42 +2813,42 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>229 (99, 496)</t>
+          <t>487 (216, 1017)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>185 (64, 439)</t>
+          <t>397 (147, 907)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>33 (13, 74)</t>
+          <t>65 (26, 143)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>30 (15, 56)</t>
+          <t>61 (32, 111)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>229 (99, 496)</t>
+          <t>487 (216, 1017)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>185 (64, 439)</t>
+          <t>397 (147, 907)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>33 (13, 74)</t>
+          <t>65 (26, 143)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>30 (15, 56)</t>
+          <t>61 (32, 111)</t>
         </is>
       </c>
     </row>
@@ -2875,42 +2875,42 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>215 (92, 476)</t>
+          <t>460 (201, 976)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>172 (58, 420)</t>
+          <t>373 (134, 868)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>32 (12, 72)</t>
+          <t>63 (25, 140)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>29 (15, 54)</t>
+          <t>59 (31, 108)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>215 (92, 476)</t>
+          <t>460 (201, 976)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>172 (58, 420)</t>
+          <t>373 (134, 868)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>32 (12, 72)</t>
+          <t>63 (25, 140)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>29 (15, 54)</t>
+          <t>59 (31, 108)</t>
         </is>
       </c>
     </row>
@@ -2937,42 +2937,42 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>203 (86, 456)</t>
+          <t>435 (189, 938)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>161 (54, 401)</t>
+          <t>351 (124, 832)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>30 (12, 70)</t>
+          <t>60 (23, 136)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>28 (14, 53)</t>
+          <t>57 (29, 105)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>203 (86, 456)</t>
+          <t>435 (189, 938)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>161 (54, 401)</t>
+          <t>351 (124, 832)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>30 (12, 70)</t>
+          <t>60 (23, 136)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>28 (14, 53)</t>
+          <t>57 (29, 105)</t>
         </is>
       </c>
     </row>
@@ -2999,42 +2999,42 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>193 (82, 439)</t>
+          <t>414 (180, 903)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>153 (51, 385)</t>
+          <t>333 (117, 799)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>29 (11, 68)</t>
+          <t>57 (22, 132)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>26 (13, 51)</t>
+          <t>54 (28, 101)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>193 (82, 439)</t>
+          <t>414 (180, 903)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>153 (51, 385)</t>
+          <t>333 (117, 799)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>29 (11, 68)</t>
+          <t>57 (22, 132)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>26 (13, 51)</t>
+          <t>54 (28, 101)</t>
         </is>
       </c>
     </row>
@@ -3061,42 +3061,42 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>184 (79, 423)</t>
+          <t>396 (172, 870)</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>145 (48, 371)</t>
+          <t>318 (112, 769)</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>27 (10, 66)</t>
+          <t>54 (21, 127)</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>25 (13, 49)</t>
+          <t>51 (26, 97)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>184 (79, 423)</t>
+          <t>396 (172, 870)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>145 (48, 371)</t>
+          <t>318 (112, 769)</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>27 (10, 66)</t>
+          <t>54 (21, 127)</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>25 (13, 49)</t>
+          <t>51 (26, 97)</t>
         </is>
       </c>
     </row>
@@ -3123,42 +3123,42 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>177 (76, 410)</t>
+          <t>381 (166, 841)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>140 (47, 359)</t>
+          <t>307 (108, 744)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>26 (10, 63)</t>
+          <t>51 (19, 123)</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>49 (24, 93)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>177 (76, 410)</t>
+          <t>381 (166, 841)</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>140 (47, 359)</t>
+          <t>307 (108, 744)</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>26 (10, 63)</t>
+          <t>51 (19, 123)</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>49 (24, 93)</t>
         </is>
       </c>
     </row>
@@ -3185,42 +3185,42 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>172 (75, 399)</t>
+          <t>369 (162, 816)</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>136 (46, 349)</t>
+          <t>298 (106, 721)</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>25 (9, 61)</t>
+          <t>49 (18, 118)</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>23 (11, 45)</t>
+          <t>46 (23, 89)</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>172 (75, 399)</t>
+          <t>369 (162, 816)</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>136 (46, 349)</t>
+          <t>298 (106, 721)</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>25 (9, 61)</t>
+          <t>49 (18, 118)</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>23 (11, 45)</t>
+          <t>46 (23, 89)</t>
         </is>
       </c>
     </row>
@@ -3247,42 +3247,42 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>168 (73, 390)</t>
+          <t>360 (159, 795)</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>134 (46, 341)</t>
+          <t>291 (105, 703)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>24 (9, 59)</t>
+          <t>46 (17, 113)</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>21 (10, 43)</t>
+          <t>44 (21, 86)</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>168 (73, 390)</t>
+          <t>360 (159, 795)</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>134 (46, 341)</t>
+          <t>291 (105, 703)</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>24 (9, 59)</t>
+          <t>46 (17, 113)</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>21 (10, 43)</t>
+          <t>44 (21, 86)</t>
         </is>
       </c>
     </row>
@@ -3309,42 +3309,42 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>165 (72, 383)</t>
+          <t>352 (156, 777)</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>132 (46, 336)</t>
+          <t>286 (104, 688)</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>22 (8, 57)</t>
+          <t>44 (16, 109)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>41 (20, 82)</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>165 (72, 383)</t>
+          <t>352 (156, 777)</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>132 (46, 336)</t>
+          <t>286 (104, 688)</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>22 (8, 57)</t>
+          <t>44 (16, 109)</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>41 (20, 82)</t>
         </is>
       </c>
     </row>
@@ -3371,42 +3371,42 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>163 (71, 378)</t>
+          <t>346 (154, 763)</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>131 (46, 332)</t>
+          <t>282 (103, 676)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>22 (8, 55)</t>
+          <t>42 (15, 105)</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>19 (9, 40)</t>
+          <t>39 (19, 79)</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>163 (71, 378)</t>
+          <t>346 (154, 763)</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>131 (46, 332)</t>
+          <t>282 (103, 676)</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>22 (8, 55)</t>
+          <t>42 (15, 105)</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>19 (9, 40)</t>
+          <t>39 (19, 79)</t>
         </is>
       </c>
     </row>
@@ -3433,42 +3433,42 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>162 (70, 375)</t>
+          <t>341 (152, 752)</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>131 (46, 329)</t>
+          <t>280 (103, 666)</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>21 (7, 53)</t>
+          <t>40 (15, 101)</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>19 (9, 39)</t>
+          <t>38 (18, 76)</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>162 (70, 375)</t>
+          <t>341 (152, 752)</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>131 (46, 329)</t>
+          <t>280 (103, 666)</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>21 (7, 53)</t>
+          <t>40 (15, 101)</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>19 (9, 39)</t>
+          <t>38 (18, 76)</t>
         </is>
       </c>
     </row>
@@ -3495,42 +3495,42 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>161 (70, 373)</t>
+          <t>337 (150, 743)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>130 (46, 328)</t>
+          <t>277 (103, 659)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>20 (7, 52)</t>
+          <t>39 (14, 98)</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>18 (9, 38)</t>
+          <t>36 (17, 74)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>161 (70, 373)</t>
+          <t>337 (150, 743)</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>130 (46, 328)</t>
+          <t>277 (103, 659)</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>20 (7, 52)</t>
+          <t>39 (14, 98)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>18 (9, 38)</t>
+          <t>36 (17, 74)</t>
         </is>
       </c>
     </row>
@@ -3557,42 +3557,42 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>278 (128, 577)</t>
+          <t>571 (271, 1117)</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>230 (89, 515)</t>
+          <t>475 (192, 1007)</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>36 (15, 79)</t>
+          <t>70 (29, 148)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>33 (17, 60)</t>
+          <t>66 (35, 115)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>278 (128, 577)</t>
+          <t>571 (271, 1117)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>230 (89, 515)</t>
+          <t>475 (192, 1007)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>36 (15, 79)</t>
+          <t>70 (29, 148)</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>33 (17, 60)</t>
+          <t>66 (35, 115)</t>
         </is>
       </c>
     </row>
@@ -3619,42 +3619,42 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>262 (118, 555)</t>
+          <t>540 (250, 1077)</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>215 (80, 494)</t>
+          <t>445 (174, 968)</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>35 (14, 78)</t>
+          <t>68 (28, 147)</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>32 (17, 60)</t>
+          <t>64 (35, 114)</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>262 (118, 555)</t>
+          <t>540 (250, 1077)</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>215 (80, 494)</t>
+          <t>445 (174, 968)</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>35 (14, 78)</t>
+          <t>68 (28, 147)</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>32 (17, 60)</t>
+          <t>64 (35, 114)</t>
         </is>
       </c>
     </row>
@@ -3681,42 +3681,42 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>247 (109, 533)</t>
+          <t>509 (231, 1036)</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>200 (73, 472)</t>
+          <t>416 (158, 927)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>34 (13, 77)</t>
+          <t>66 (27, 145)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>31 (16, 58)</t>
+          <t>63 (33, 112)</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>247 (109, 533)</t>
+          <t>509 (231, 1036)</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>200 (73, 472)</t>
+          <t>416 (158, 927)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>34 (13, 77)</t>
+          <t>66 (27, 145)</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>31 (16, 58)</t>
+          <t>63 (33, 112)</t>
         </is>
       </c>
     </row>
@@ -3743,42 +3743,42 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>232 (102, 511)</t>
+          <t>480 (215, 995)</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>188 (66, 452)</t>
+          <t>390 (144, 889)</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>33 (13, 75)</t>
+          <t>64 (26, 142)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>30 (15, 57)</t>
+          <t>61 (32, 109)</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>232 (102, 511)</t>
+          <t>480 (215, 995)</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>188 (66, 452)</t>
+          <t>390 (144, 889)</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>33 (13, 75)</t>
+          <t>64 (26, 142)</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>30 (15, 57)</t>
+          <t>61 (32, 109)</t>
         </is>
       </c>
     </row>
@@ -3805,42 +3805,42 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>220 (96, 491)</t>
+          <t>454 (201, 956)</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>177 (62, 433)</t>
+          <t>368 (133, 852)</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>31 (12, 73)</t>
+          <t>61 (24, 138)</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>29 (15, 55)</t>
+          <t>58 (31, 106)</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>220 (96, 491)</t>
+          <t>454 (201, 956)</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>177 (62, 433)</t>
+          <t>368 (133, 852)</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>31 (12, 73)</t>
+          <t>61 (24, 138)</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>29 (15, 55)</t>
+          <t>58 (31, 106)</t>
         </is>
       </c>
     </row>
@@ -3867,42 +3867,42 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>209 (91, 472)</t>
+          <t>431 (190, 920)</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>167 (58, 416)</t>
+          <t>348 (124, 818)</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>30 (11, 71)</t>
+          <t>58 (23, 133)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>28 (14, 53)</t>
+          <t>55 (29, 102)</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>209 (91, 472)</t>
+          <t>431 (190, 920)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>167 (58, 416)</t>
+          <t>348 (124, 818)</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>30 (11, 71)</t>
+          <t>58 (23, 133)</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>28 (14, 53)</t>
+          <t>55 (29, 102)</t>
         </is>
       </c>
     </row>
@@ -3929,42 +3929,42 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>200 (87, 456)</t>
+          <t>411 (181, 886)</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>160 (55, 401)</t>
+          <t>332 (118, 787)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>29 (11, 68)</t>
+          <t>55 (21, 129)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>26 (13, 51)</t>
+          <t>53 (27, 98)</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>200 (87, 456)</t>
+          <t>411 (181, 886)</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>160 (55, 401)</t>
+          <t>332 (118, 787)</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>29 (11, 68)</t>
+          <t>55 (21, 129)</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>26 (13, 51)</t>
+          <t>53 (27, 98)</t>
         </is>
       </c>
     </row>
@@ -3991,42 +3991,42 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>192 (84, 441)</t>
+          <t>394 (174, 857)</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>154 (54, 388)</t>
+          <t>318 (113, 761)</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>27 (10, 66)</t>
+          <t>52 (20, 124)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>25 (12, 49)</t>
+          <t>50 (26, 94)</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>192 (84, 441)</t>
+          <t>394 (174, 857)</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>154 (54, 388)</t>
+          <t>318 (113, 761)</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>27 (10, 66)</t>
+          <t>52 (20, 124)</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>25 (12, 49)</t>
+          <t>50 (26, 94)</t>
         </is>
       </c>
     </row>
@@ -4053,42 +4053,42 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>186 (82, 429)</t>
+          <t>380 (167, 831)</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>149 (53, 377)</t>
+          <t>307 (109, 737)</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>26 (9, 64)</t>
+          <t>50 (19, 119)</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>47 (24, 90)</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>186 (82, 429)</t>
+          <t>380 (167, 831)</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>149 (53, 377)</t>
+          <t>307 (109, 737)</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>26 (9, 64)</t>
+          <t>50 (19, 119)</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>24 (12, 47)</t>
+          <t>47 (24, 90)</t>
         </is>
       </c>
     </row>
@@ -4115,42 +4115,42 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>182 (80, 418)</t>
+          <t>368 (162, 807)</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>146 (52, 368)</t>
+          <t>298 (107, 715)</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>25 (9, 61)</t>
+          <t>47 (18, 115)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>22 (11, 45)</t>
+          <t>45 (22, 87)</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>182 (80, 418)</t>
+          <t>368 (162, 807)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>146 (52, 368)</t>
+          <t>298 (107, 715)</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>25 (9, 61)</t>
+          <t>47 (18, 115)</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>22 (11, 45)</t>
+          <t>45 (22, 87)</t>
         </is>
       </c>
     </row>
@@ -4177,42 +4177,42 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>178 (79, 410)</t>
+          <t>358 (158, 787)</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>143 (51, 360)</t>
+          <t>291 (104, 697)</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>24 (9, 59)</t>
+          <t>45 (17, 110)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>21 (10, 43)</t>
+          <t>42 (21, 83)</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>178 (79, 410)</t>
+          <t>358 (158, 787)</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>143 (51, 360)</t>
+          <t>291 (104, 697)</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>24 (9, 59)</t>
+          <t>45 (17, 110)</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>21 (10, 43)</t>
+          <t>42 (21, 83)</t>
         </is>
       </c>
     </row>
@@ -4239,42 +4239,42 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>175 (77, 403)</t>
+          <t>349 (154, 769)</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>141 (51, 355)</t>
+          <t>284 (102, 682)</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>22 (8, 57)</t>
+          <t>42 (16, 106)</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>40 (20, 79)</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>175 (77, 403)</t>
+          <t>349 (154, 769)</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>141 (51, 355)</t>
+          <t>284 (102, 682)</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>22 (8, 57)</t>
+          <t>42 (16, 106)</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>20 (10, 42)</t>
+          <t>40 (20, 79)</t>
         </is>
       </c>
     </row>
@@ -4301,42 +4301,42 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>172 (76, 398)</t>
+          <t>341 (150, 755)</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>140 (50, 350)</t>
+          <t>279 (101, 670)</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>22 (8, 55)</t>
+          <t>40 (15, 102)</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>19 (9, 40)</t>
+          <t>38 (19, 76)</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>172 (76, 398)</t>
+          <t>341 (150, 755)</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>140 (50, 350)</t>
+          <t>279 (101, 670)</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>22 (8, 55)</t>
+          <t>40 (15, 102)</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>19 (9, 40)</t>
+          <t>38 (19, 76)</t>
         </is>
       </c>
     </row>
@@ -4363,42 +4363,42 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>170 (75, 393)</t>
+          <t>334 (147, 742)</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>139 (50, 347)</t>
+          <t>274 (99, 659)</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>21 (8, 54)</t>
+          <t>39 (14, 98)</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>19 (9, 39)</t>
+          <t>37 (18, 74)</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>170 (75, 393)</t>
+          <t>334 (147, 742)</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>139 (50, 347)</t>
+          <t>274 (99, 659)</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>21 (8, 54)</t>
+          <t>39 (14, 98)</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>19 (9, 39)</t>
+          <t>37 (18, 74)</t>
         </is>
       </c>
     </row>

</xml_diff>